<commit_message>
Add support for candidate taxi times
</commit_message>
<xml_diff>
--- a/hr-buddy-server/src/main/resources/static/example-planning.xlsx
+++ b/hr-buddy-server/src/main/resources/static/example-planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_clones\hr-buddy\agenda-generator\samples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="11_3EC5D3A22BC07B6FEB3A426B864E09A0599994B3" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{C1FB299D-434D-47F6-B8C6-68433090600D}"/>
+  <xr:revisionPtr revIDLastSave="59" documentId="11_3EC5D3A22BC07B6FEB3A426B864E09A0599994B3" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{FC0C2612-CA8C-4782-9784-0DA9175B8C0B}"/>
   <bookViews>
     <workbookView xWindow="9450" yWindow="3240" windowWidth="12330" windowHeight="6060" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="60">
   <si>
     <t>RECRUITMENT DAY AIR-DGA 2018-09-05</t>
   </si>
@@ -205,24 +205,6 @@
   </si>
   <si>
     <t>Evening taxi</t>
-  </si>
-  <si>
-    <t>8h10</t>
-  </si>
-  <si>
-    <t>17h30</t>
-  </si>
-  <si>
-    <t>8h00</t>
-  </si>
-  <si>
-    <t>17h15</t>
-  </si>
-  <si>
-    <t>7h50</t>
-  </si>
-  <si>
-    <t>17h00</t>
   </si>
 </sst>
 </file>
@@ -487,7 +469,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -538,9 +520,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="20" fontId="4" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -585,47 +564,47 @@
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="15" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="20" fontId="11" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -989,13 +968,13 @@
   <sheetData>
     <row r="2" spans="1:8" ht="15.75">
       <c r="A2" s="3"/>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="41"/>
-      <c r="D2" s="41"/>
-      <c r="E2" s="41"/>
-      <c r="F2" s="41"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
     </row>
     <row r="3" spans="1:8" ht="15">
       <c r="A3" s="3"/>
@@ -1008,13 +987,13 @@
     </row>
     <row r="4" spans="1:8" ht="15">
       <c r="A4" s="3"/>
-      <c r="B4" s="38" t="s">
+      <c r="B4" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="40"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="42"/>
     </row>
     <row r="5" spans="1:8" ht="15">
       <c r="A5" s="3"/>
@@ -1026,7 +1005,7 @@
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:8" ht="15.75">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="28" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="5" t="s">
@@ -1046,41 +1025,41 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="15.75">
-      <c r="A7" s="31" t="s">
+      <c r="A7" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="30" t="s">
+      <c r="C7" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="30" t="s">
+      <c r="D7" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="30" t="s">
+      <c r="F7" s="29" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75">
-      <c r="A8" s="31" t="s">
+      <c r="A8" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="29" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="30"/>
-      <c r="D8" s="30" t="s">
+      <c r="C8" s="29"/>
+      <c r="D8" s="29" t="s">
         <v>15</v>
       </c>
-      <c r="E8" s="30"/>
-      <c r="F8" s="30"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="29"/>
     </row>
     <row r="9" spans="1:8" ht="15.75">
-      <c r="A9" s="32" t="s">
+      <c r="A9" s="31" t="s">
         <v>16</v>
       </c>
       <c r="B9" s="7" t="s">
@@ -1106,9 +1085,9 @@
       <c r="B10" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="22"/>
-      <c r="D10" s="22"/>
-      <c r="E10" s="22"/>
+      <c r="C10" s="21"/>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
       <c r="F10" s="12" t="s">
         <v>23</v>
       </c>
@@ -1118,12 +1097,12 @@
       <c r="A11" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="22"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
       <c r="F11" s="14" t="s">
         <v>22</v>
       </c>
@@ -1132,13 +1111,13 @@
       <c r="A12" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="22"/>
-      <c r="C12" s="22"/>
+      <c r="B12" s="21"/>
+      <c r="C12" s="21"/>
       <c r="D12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="22"/>
-      <c r="F12" s="24" t="s">
+      <c r="E12" s="21"/>
+      <c r="F12" s="23" t="s">
         <v>27</v>
       </c>
     </row>
@@ -1146,10 +1125,10 @@
       <c r="A13" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="22"/>
-      <c r="E13" s="24" t="s">
+      <c r="B13" s="21"/>
+      <c r="C13" s="21"/>
+      <c r="D13" s="21"/>
+      <c r="E13" s="23" t="s">
         <v>27</v>
       </c>
       <c r="F13" s="13" t="s">
@@ -1158,26 +1137,26 @@
       <c r="H13" s="16"/>
     </row>
     <row r="14" spans="1:8" ht="15.75">
-      <c r="A14" s="28"/>
-      <c r="B14" s="42" t="s">
+      <c r="A14" s="27"/>
+      <c r="B14" s="44" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="43"/>
-      <c r="E14" s="43"/>
-      <c r="F14" s="44"/>
+      <c r="C14" s="45"/>
+      <c r="D14" s="45"/>
+      <c r="E14" s="45"/>
+      <c r="F14" s="46"/>
     </row>
     <row r="15" spans="1:8" ht="15.75">
       <c r="A15" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="35" t="s">
+      <c r="B15" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="36"/>
-      <c r="D15" s="36"/>
-      <c r="E15" s="36"/>
-      <c r="F15" s="37"/>
+      <c r="C15" s="38"/>
+      <c r="D15" s="38"/>
+      <c r="E15" s="38"/>
+      <c r="F15" s="39"/>
     </row>
     <row r="16" spans="1:8" ht="15">
       <c r="A16" s="3"/>
@@ -1188,7 +1167,7 @@
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
-      <c r="F17" s="21" t="s">
+      <c r="F17" s="20" t="s">
         <v>32</v>
       </c>
     </row>
@@ -1207,13 +1186,13 @@
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
-      <c r="F19" s="21" t="s">
+      <c r="F19" s="20" t="s">
         <v>33</v>
       </c>
       <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:13" ht="15.75">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="28" t="s">
         <v>2</v>
       </c>
       <c r="B20" s="6" t="s">
@@ -1225,10 +1204,10 @@
       <c r="F20" s="9"/>
     </row>
     <row r="21" spans="1:13" ht="14.25" customHeight="1">
-      <c r="A21" s="31" t="s">
+      <c r="A21" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="29" t="s">
         <v>35</v>
       </c>
       <c r="C21" s="9"/>
@@ -1242,13 +1221,13 @@
       <c r="B22" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="20" t="s">
+      <c r="D22" s="19" t="s">
         <v>36</v>
       </c>
       <c r="E22" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="F22" s="19"/>
+      <c r="F22" s="18"/>
       <c r="G22" s="2" t="s">
         <v>37</v>
       </c>
@@ -1257,19 +1236,19 @@
       <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B23" s="24" t="s">
+      <c r="B23" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="D23" s="20"/>
+      <c r="D23" s="19"/>
       <c r="E23" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="F23" s="19"/>
+      <c r="F23" s="18"/>
       <c r="G23" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="H23" s="20"/>
-      <c r="I23" s="20"/>
+      <c r="H23" s="19"/>
+      <c r="I23" s="19"/>
     </row>
     <row r="24" spans="1:13" ht="15.75">
       <c r="A24" s="8" t="s">
@@ -1278,13 +1257,13 @@
       <c r="B24" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="19" t="s">
         <v>39</v>
       </c>
       <c r="E24" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F24" s="19"/>
+      <c r="F24" s="18"/>
       <c r="G24" s="2" t="s">
         <v>40</v>
       </c>
@@ -1296,13 +1275,13 @@
       <c r="B25" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="E25" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="F25" s="19"/>
+      <c r="F25" s="18"/>
       <c r="G25" s="2" t="s">
         <v>38</v>
       </c>
@@ -1314,14 +1293,14 @@
       <c r="B26" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="20"/>
-      <c r="E26" s="20"/>
-      <c r="F26" s="20"/>
-      <c r="G26" s="20"/>
+      <c r="D26" s="19"/>
+      <c r="E26" s="19"/>
+      <c r="F26" s="19"/>
+      <c r="G26" s="19"/>
     </row>
     <row r="27" spans="1:13" ht="15.75" customHeight="1">
-      <c r="A27" s="28"/>
-      <c r="B27" s="27" t="s">
+      <c r="A27" s="27"/>
+      <c r="B27" s="26" t="s">
         <v>29</v>
       </c>
       <c r="C27" s="9"/>
@@ -1332,7 +1311,7 @@
       <c r="A28" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="23" t="s">
+      <c r="B28" s="22" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="9"/>
@@ -1340,7 +1319,7 @@
     </row>
     <row r="29" spans="1:13" ht="15.75">
       <c r="C29" s="9"/>
-      <c r="D29" s="25" t="s">
+      <c r="D29" s="24" t="s">
         <v>41</v>
       </c>
       <c r="M29" s="15"/>
@@ -1350,10 +1329,10 @@
       <c r="D30" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="F30" s="26"/>
+      <c r="F30" s="25"/>
     </row>
     <row r="31" spans="1:13" ht="15.75">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="28" t="s">
         <v>2</v>
       </c>
       <c r="B31" s="6" t="s">
@@ -1363,13 +1342,13 @@
       <c r="D31" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="26"/>
+      <c r="F31" s="25"/>
     </row>
     <row r="32" spans="1:13" ht="15.75">
-      <c r="A32" s="31" t="s">
+      <c r="A32" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="29" t="s">
         <v>45</v>
       </c>
       <c r="C32" s="9"/>
@@ -1399,7 +1378,7 @@
       <c r="A35" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B35" s="24" t="s">
+      <c r="B35" s="23" t="s">
         <v>27</v>
       </c>
       <c r="C35" s="9"/>
@@ -1426,8 +1405,8 @@
       <c r="D37" s="9"/>
     </row>
     <row r="38" spans="1:4" ht="15.75">
-      <c r="A38" s="28"/>
-      <c r="B38" s="27" t="s">
+      <c r="A38" s="27"/>
+      <c r="B38" s="26" t="s">
         <v>29</v>
       </c>
       <c r="C38" s="9"/>
@@ -1437,7 +1416,7 @@
       <c r="A39" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B39" s="23" t="s">
+      <c r="B39" s="22" t="s">
         <v>31</v>
       </c>
       <c r="C39" s="9"/>
@@ -1487,15 +1466,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="34" t="s">
+      <c r="A1" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="33">
+      <c r="B1" s="32">
         <v>43228</v>
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="34" t="s">
+      <c r="A2" s="33" t="s">
         <v>49</v>
       </c>
       <c r="B2" t="s">
@@ -1503,7 +1482,7 @@
       </c>
     </row>
     <row r="3" spans="1:2">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="33" t="s">
         <v>51</v>
       </c>
       <c r="B3" t="s">
@@ -1511,7 +1490,7 @@
       </c>
     </row>
     <row r="4" spans="1:2">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="33" t="s">
         <v>53</v>
       </c>
       <c r="B4" t="s">
@@ -1519,7 +1498,7 @@
       </c>
     </row>
     <row r="5" spans="1:2">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="33" t="s">
         <v>55</v>
       </c>
       <c r="B5" t="s">
@@ -1543,7 +1522,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <selection activeCell="A6" sqref="A6:XFD6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25"/>
@@ -1559,14 +1538,14 @@
     <col min="9" max="16384" width="8.85546875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="46" customFormat="1" ht="15">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:3" s="35" customFormat="1" ht="15">
+      <c r="A1" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="45" t="s">
+      <c r="B1" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C1" s="45" t="s">
+      <c r="C1" s="34" t="s">
         <v>59</v>
       </c>
     </row>
@@ -1574,44 +1553,44 @@
       <c r="A2" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="B2" s="47" t="s">
-        <v>60</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>61</v>
+      <c r="B2" s="36">
+        <v>0.34027777777777773</v>
+      </c>
+      <c r="C2" s="47">
+        <v>0.72916666666666663</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15">
       <c r="A3" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="47" t="s">
-        <v>62</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>63</v>
+      <c r="B3" s="36">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C3" s="47">
+        <v>0.71875</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15">
       <c r="A4" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="47" t="s">
-        <v>64</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>65</v>
+      <c r="B4" s="36">
+        <v>0.3263888888888889</v>
+      </c>
+      <c r="C4" s="47">
+        <v>0.72916666666666663</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15">
       <c r="A5" s="17" t="s">
         <v>27</v>
       </c>
-      <c r="B5" s="48" t="s">
-        <v>62</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>65</v>
+      <c r="B5" s="36">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="C5" s="47">
+        <v>0.70833333333333337</v>
       </c>
     </row>
     <row r="8" spans="1:3">

</xml_diff>

<commit_message>
Make taxi times optional
Resolves:
https://github.com/joffrey-bion/hr-buddy/issues/4
</commit_message>
<xml_diff>
--- a/hr-buddy-server/src/main/resources/static/example-planning.xlsx
+++ b/hr-buddy-server/src/main/resources/static/example-planning.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20919"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_clones\hr-buddy\agenda-generator\samples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\projects\hr-buddy\hr-buddy-server\src\main\resources\static\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="59" documentId="11_3EC5D3A22BC07B6FEB3A426B864E09A0599994B3" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{FC0C2612-CA8C-4782-9784-0DA9175B8C0B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{0D3B129D-38F7-4D86-8B39-10C221A3A854}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9450" yWindow="3240" windowWidth="12330" windowHeight="6060" firstSheet="2" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Planning!$A$1:$F$26</definedName>
   </definedNames>
-  <calcPr calcId="179020"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
@@ -214,7 +214,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="h:mm;@"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -573,38 +573,38 @@
     <xf numFmtId="20" fontId="11" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="20" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="12" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="12" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="12" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -949,11 +949,11 @@
   </sheetPr>
   <dimension ref="A2:M46"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+    <sheetView topLeftCell="A15" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
     <col min="2" max="4" width="43.5703125" style="2" customWidth="1"/>
@@ -966,17 +966,17 @@
     <col min="13" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:8" ht="15.75">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3"/>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="44" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-    </row>
-    <row r="3" spans="1:8" ht="15">
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+    </row>
+    <row r="3" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="3"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -985,17 +985,17 @@
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="15">
+    <row r="4" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="3"/>
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
-      <c r="E4" s="41"/>
-      <c r="F4" s="42"/>
-    </row>
-    <row r="5" spans="1:8" ht="15">
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="43"/>
+    </row>
+    <row r="5" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1004,7 +1004,7 @@
       <c r="F5" s="4"/>
       <c r="G5" s="4"/>
     </row>
-    <row r="6" spans="1:8" ht="15.75">
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="28" t="s">
         <v>2</v>
       </c>
@@ -1024,7 +1024,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="15.75">
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" s="30" t="s">
         <v>8</v>
       </c>
@@ -1044,7 +1044,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15.75">
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A8" s="30" t="s">
         <v>13</v>
       </c>
@@ -1058,7 +1058,7 @@
       <c r="E8" s="29"/>
       <c r="F8" s="29"/>
     </row>
-    <row r="9" spans="1:8" ht="15.75">
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9" s="31" t="s">
         <v>16</v>
       </c>
@@ -1078,7 +1078,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="15.75">
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A10" s="8" t="s">
         <v>21</v>
       </c>
@@ -1093,7 +1093,7 @@
       </c>
       <c r="H10" s="16"/>
     </row>
-    <row r="11" spans="1:8" ht="15.75">
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
         <v>24</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="15.75" customHeight="1">
+    <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8" t="s">
         <v>26</v>
       </c>
@@ -1121,7 +1121,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="15.75">
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
         <v>28</v>
       </c>
@@ -1136,32 +1136,32 @@
       </c>
       <c r="H13" s="16"/>
     </row>
-    <row r="14" spans="1:8" ht="15.75">
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A14" s="27"/>
-      <c r="B14" s="44" t="s">
+      <c r="B14" s="45" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="45"/>
-      <c r="D14" s="45"/>
-      <c r="E14" s="45"/>
-      <c r="F14" s="46"/>
-    </row>
-    <row r="15" spans="1:8" ht="15.75">
+      <c r="C14" s="46"/>
+      <c r="D14" s="46"/>
+      <c r="E14" s="46"/>
+      <c r="F14" s="47"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="38" t="s">
         <v>31</v>
       </c>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="39"/>
-    </row>
-    <row r="16" spans="1:8" ht="15">
+      <c r="C15" s="39"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="39"/>
+      <c r="F15" s="40"/>
+    </row>
+    <row r="16" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" s="3"/>
     </row>
-    <row r="17" spans="1:13" ht="15.75">
+    <row r="17" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A17" s="3"/>
       <c r="B17" s="9"/>
       <c r="C17" s="9"/>
@@ -1171,7 +1171,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:13" ht="15.75">
+    <row r="18" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" s="3"/>
       <c r="B18" s="9"/>
       <c r="C18" s="9"/>
@@ -1180,7 +1180,7 @@
       <c r="F18" s="9"/>
       <c r="G18" s="4"/>
     </row>
-    <row r="19" spans="1:13" ht="15.75">
+    <row r="19" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" s="3"/>
       <c r="B19" s="9"/>
       <c r="C19" s="9"/>
@@ -1191,7 +1191,7 @@
       </c>
       <c r="G19" s="4"/>
     </row>
-    <row r="20" spans="1:13" ht="15.75">
+    <row r="20" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" s="28" t="s">
         <v>2</v>
       </c>
@@ -1203,7 +1203,7 @@
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
     </row>
-    <row r="21" spans="1:13" ht="14.25" customHeight="1">
+    <row r="21" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="30" t="s">
         <v>8</v>
       </c>
@@ -1214,7 +1214,7 @@
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
     </row>
-    <row r="22" spans="1:13" ht="14.25" customHeight="1">
+    <row r="22" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>16</v>
       </c>
@@ -1232,7 +1232,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="23" spans="1:13" ht="14.25" customHeight="1">
+    <row r="23" spans="1:13" ht="14.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="8" t="s">
         <v>21</v>
       </c>
@@ -1250,7 +1250,7 @@
       <c r="H23" s="19"/>
       <c r="I23" s="19"/>
     </row>
-    <row r="24" spans="1:13" ht="15.75">
+    <row r="24" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A24" s="8" t="s">
         <v>24</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:13" ht="15.75" customHeight="1">
+    <row r="25" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="8" t="s">
         <v>26</v>
       </c>
@@ -1286,7 +1286,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15.75">
+    <row r="26" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A26" s="8" t="s">
         <v>28</v>
       </c>
@@ -1298,7 +1298,7 @@
       <c r="F26" s="19"/>
       <c r="G26" s="19"/>
     </row>
-    <row r="27" spans="1:13" ht="15.75" customHeight="1">
+    <row r="27" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="27"/>
       <c r="B27" s="26" t="s">
         <v>29</v>
@@ -1307,7 +1307,7 @@
       <c r="D27" s="9"/>
       <c r="M27" s="15"/>
     </row>
-    <row r="28" spans="1:13" ht="15.75">
+    <row r="28" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" s="8" t="s">
         <v>30</v>
       </c>
@@ -1317,21 +1317,21 @@
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
     </row>
-    <row r="29" spans="1:13" ht="15.75">
+    <row r="29" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C29" s="9"/>
       <c r="D29" s="24" t="s">
         <v>41</v>
       </c>
       <c r="M29" s="15"/>
     </row>
-    <row r="30" spans="1:13" ht="15.75">
+    <row r="30" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C30" s="9"/>
       <c r="D30" s="4" t="s">
         <v>42</v>
       </c>
       <c r="F30" s="25"/>
     </row>
-    <row r="31" spans="1:13" ht="15.75">
+    <row r="31" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" s="28" t="s">
         <v>2</v>
       </c>
@@ -1344,7 +1344,7 @@
       </c>
       <c r="F31" s="25"/>
     </row>
-    <row r="32" spans="1:13" ht="15.75">
+    <row r="32" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A32" s="30" t="s">
         <v>8</v>
       </c>
@@ -1354,7 +1354,7 @@
       <c r="C32" s="9"/>
       <c r="D32" s="9"/>
     </row>
-    <row r="33" spans="1:4" ht="15.75">
+    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" s="7" t="s">
         <v>16</v>
       </c>
@@ -1364,7 +1364,7 @@
       <c r="C33" s="9"/>
       <c r="D33" s="9"/>
     </row>
-    <row r="34" spans="1:4" ht="15.75">
+    <row r="34" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A34" s="8" t="s">
         <v>21</v>
       </c>
@@ -1374,7 +1374,7 @@
       <c r="C34" s="9"/>
       <c r="D34" s="9"/>
     </row>
-    <row r="35" spans="1:4" ht="15.75">
+    <row r="35" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A35" s="8" t="s">
         <v>24</v>
       </c>
@@ -1384,7 +1384,7 @@
       <c r="C35" s="9"/>
       <c r="D35" s="9"/>
     </row>
-    <row r="36" spans="1:4" ht="15.75">
+    <row r="36" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A36" s="8" t="s">
         <v>26</v>
       </c>
@@ -1394,7 +1394,7 @@
       <c r="C36" s="9"/>
       <c r="D36" s="9"/>
     </row>
-    <row r="37" spans="1:4" ht="15.75">
+    <row r="37" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A37" s="8" t="s">
         <v>28</v>
       </c>
@@ -1404,7 +1404,7 @@
       <c r="C37" s="9"/>
       <c r="D37" s="9"/>
     </row>
-    <row r="38" spans="1:4" ht="15.75">
+    <row r="38" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A38" s="27"/>
       <c r="B38" s="26" t="s">
         <v>29</v>
@@ -1412,7 +1412,7 @@
       <c r="C38" s="9"/>
       <c r="D38" s="9"/>
     </row>
-    <row r="39" spans="1:4" ht="15.75">
+    <row r="39" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A39" s="8" t="s">
         <v>30</v>
       </c>
@@ -1422,15 +1422,15 @@
       <c r="C39" s="9"/>
       <c r="D39" s="9"/>
     </row>
-    <row r="40" spans="1:4" ht="15.75">
+    <row r="40" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C40" s="9"/>
       <c r="D40" s="9"/>
     </row>
-    <row r="41" spans="1:4" ht="15.75">
+    <row r="41" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="C41" s="9"/>
       <c r="D41" s="9"/>
     </row>
-    <row r="46" spans="1:4">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A46" s="1" t="s">
         <v>47</v>
       </c>
@@ -1454,18 +1454,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.7109375" customWidth="1"/>
     <col min="2" max="2" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="33" t="s">
         <v>48</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>43228</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="33" t="s">
         <v>49</v>
       </c>
@@ -1481,7 +1481,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="33" t="s">
         <v>51</v>
       </c>
@@ -1489,7 +1489,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="33" t="s">
         <v>53</v>
       </c>
@@ -1497,7 +1497,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="33" t="s">
         <v>55</v>
       </c>
@@ -1521,11 +1521,11 @@
   </sheetPr>
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="41.5703125" style="11" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5703125" style="10" customWidth="1"/>
@@ -1538,7 +1538,7 @@
     <col min="9" max="16384" width="8.85546875" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="35" customFormat="1" ht="15">
+    <row r="1" spans="1:3" s="35" customFormat="1" ht="15" x14ac:dyDescent="0.25">
       <c r="A1" s="34" t="s">
         <v>57</v>
       </c>
@@ -1549,72 +1549,68 @@
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>23</v>
       </c>
       <c r="B2" s="36">
         <v>0.34027777777777773</v>
       </c>
-      <c r="C2" s="47">
+      <c r="C2" s="37">
         <v>0.72916666666666663</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="17" t="s">
         <v>25</v>
       </c>
       <c r="B3" s="36">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C3" s="47">
+      <c r="C3" s="37">
         <v>0.71875</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="36">
-        <v>0.3263888888888889</v>
-      </c>
-      <c r="C4" s="47">
+      <c r="B4" s="36"/>
+      <c r="C4" s="37">
         <v>0.72916666666666663</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="17" t="s">
         <v>27</v>
       </c>
       <c r="B5" s="36">
         <v>0.33333333333333331</v>
       </c>
-      <c r="C5" s="47">
-        <v>0.70833333333333337</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="C5" s="37"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="10"/>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="10"/>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
     </row>
   </sheetData>

</xml_diff>